<commit_message>
new format- html_clean final.
</commit_message>
<xml_diff>
--- a/Rawdata/GDPDloxPintHANeoR_oligos.xlsx
+++ b/Rawdata/GDPDloxPintHANeoR_oligos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ArmorATD/Dropbox (The Francis Crick)/Data/RStudio/InteractivePaper/Rawdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramapra/Dropbox (The Francis Crick)/Data/RStudio/GDPDxcute/Rawdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12348957-2029-B344-86D1-7AA1C3AAA965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD94F4D-3E81-8C42-A487-24EA9E17E6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="600" windowWidth="27640" windowHeight="16940" xr2:uid="{1E4E001C-A525-D94A-A983-3AA213B69B7C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Primer/Oligo Name</t>
   </si>
@@ -87,13 +87,28 @@
   </si>
   <si>
     <t>TCTTCTTCAGTATTTATATTTGTATCAAGG</t>
+  </si>
+  <si>
+    <t>PF3D7_1406300-cKO-exc_5</t>
+  </si>
+  <si>
+    <t>ATATTATACACGTGTACACATTATAAC</t>
+  </si>
+  <si>
+    <t>excision</t>
+  </si>
+  <si>
+    <t>PF3D7_1406300-cKO-exc_6</t>
+  </si>
+  <si>
+    <t>gcatcaccttcaccctctcc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +124,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -148,14 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -166,6 +183,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89278FDF-61B3-6A43-898C-5300C5A4ADD3}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,69 +526,81 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="388" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>